<commit_message>
A1#111DEDALUS0000 DEDALUS TCWA 10.6 - Quinta pull request per modifica report-checklist (colonna "gestione errore")
Quinta pull request per modifica report-checklist (colonna "gestione errore")
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS/TCWA/10.6/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS/TCWA/10.6/report-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Accreditamento TCWA\pdf - quarto invio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Accreditamento TCWA\GATEWAY - OK\A1#111DEDALUS0000\DEDALUS\TCWA\10.6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838434DF-4A69-4E61-A39F-6A91EE4E6CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46470C91-33D7-4873-9DBF-DDDB0EBC6ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15750" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Prerequisiti" sheetId="1" r:id="rId1"/>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="145">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -536,13 +536,7 @@
     <t>NO</t>
   </si>
   <si>
-    <t>Viene segnalato all'utente un errore di timeout, chidendo conferma se proseguire con la validazione del documento o riprovare più tardi</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>Viene segnalato all'utente l'errore, chidendo conferma se proseguire con la validazione del documento o annullare l'operazione per correggere il problema</t>
   </si>
   <si>
     <t>Dedalus</t>
@@ -699,6 +693,15 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.160.4.4.b0f3ffcf25ce2aafc7dc901e2febc51f43837f4ca0fe3b6d1b02194e9047b6db.e1dd3a20fd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene segnalato all'utente l'errore, chiedendo conferma se proseguire con l'invio del documento o se annullare l'operazione per correggere il problema. Il sistema di CCE segnala l'errore affinchè l'utente possa correggere i dati errati/mancanti o, se impossibilitato a farlo per mancanza di autorizzazioni specifiche, segnalarlo al personale del CED affinchè intervenga direttamente. Il perimetro di azione dell'utente della CCE, ovvero la sua capacità di risoluzione di eventuali errori, dipende dalla configurazione dell'impianto e dalle policy concordate con il cliente e con i gestori dei SW dai quali vengono recuperati i dati (es. MPI, ADT, CUP, etc)</t>
+  </si>
+  <si>
+    <t>Viene segnalato all'utente l'errore, chiedendo conferma se proseguire con l'invio del documento o annullare l'operazione per correggere il problema. La gestione dell'errore è a carico del sistema di pubblicazione, ovvero alla piattaforma ESB in uso. Trattandosi di errore non dipendente dall'operatore, la sua correzione sarà a carico del gestore del sistema pubblicante (fornitore e/o CED ospedaliero)</t>
+  </si>
+  <si>
+    <t>Viene segnalato all'utente l'errore, chiedendo conferma se proseguire con l'invio del documento o annullare l'operazione per correggere il problema. La gestione dell'errore è a carico del sistema di pubblicazione, ovvero alla piattaforma ESB in uso, che può gestire sia successivi retry automatici (code) o il reinvio manuale a carico di operatore tecnico autorizzato (CED/assistenza).</t>
   </si>
 </sst>
 </file>
@@ -1579,11 +1582,11 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="194.140625" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="194.109375" customWidth="1"/>
+    <col min="3" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -2649,25 +2652,25 @@
   <dimension ref="A1:O873"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="F24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" customWidth="1"/>
-    <col min="5" max="5" width="104.7109375" customWidth="1"/>
-    <col min="6" max="9" width="33.28515625" customWidth="1"/>
-    <col min="10" max="11" width="27.28515625" customWidth="1"/>
-    <col min="12" max="12" width="33.28515625" customWidth="1"/>
-    <col min="13" max="14" width="36.42578125" customWidth="1"/>
-    <col min="15" max="15" width="98.5703125" customWidth="1"/>
-    <col min="16" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="46.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="63.88671875" customWidth="1"/>
+    <col min="5" max="5" width="104.6640625" customWidth="1"/>
+    <col min="6" max="9" width="33.33203125" customWidth="1"/>
+    <col min="10" max="11" width="27.33203125" customWidth="1"/>
+    <col min="12" max="12" width="33.33203125" customWidth="1"/>
+    <col min="13" max="14" width="36.44140625" customWidth="1"/>
+    <col min="15" max="15" width="98.5546875" customWidth="1"/>
+    <col min="16" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2682,13 +2685,13 @@
       <c r="N1" s="9"/>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" ht="18.75">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" s="46" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="47"/>
       <c r="C2" s="48" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="47"/>
       <c r="F2" s="7"/>
@@ -2702,13 +2705,13 @@
       <c r="N2" s="9"/>
       <c r="O2" s="6"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="15.6">
       <c r="A3" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="50"/>
       <c r="C3" s="55" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3" s="47"/>
       <c r="F3" s="7"/>
@@ -2722,11 +2725,11 @@
       <c r="N3" s="9"/>
       <c r="O3" s="6"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.6">
       <c r="A4" s="51"/>
       <c r="B4" s="52"/>
       <c r="C4" s="55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D4" s="47"/>
       <c r="E4" s="2"/>
@@ -2741,11 +2744,11 @@
       <c r="N4" s="9"/>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.6">
       <c r="A5" s="53"/>
       <c r="B5" s="54"/>
       <c r="C5" s="55" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D5" s="47"/>
       <c r="F5" s="7"/>
@@ -2789,7 +2792,7 @@
       <c r="N7" s="9"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1">
+    <row r="8" spans="1:15" ht="15" thickBot="1">
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -2801,7 +2804,7 @@
       <c r="N8" s="9"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="19.5" thickBot="1">
+    <row r="9" spans="1:15" ht="18.600000000000001" thickBot="1">
       <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
@@ -2848,7 +2851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="150.75" thickBot="1">
+    <row r="10" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A10" s="14">
         <v>6</v>
       </c>
@@ -2868,13 +2871,13 @@
         <v>45042</v>
       </c>
       <c r="G10" s="39" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="38" t="s">
         <v>99</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="I10" s="38" t="s">
-        <v>101</v>
       </c>
       <c r="J10" s="19"/>
       <c r="K10" s="19" t="s">
@@ -2885,7 +2888,7 @@
       <c r="N10" s="20"/>
       <c r="O10" s="21"/>
     </row>
-    <row r="11" spans="1:15" ht="150.75" thickBot="1">
+    <row r="11" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A11" s="14">
         <v>7</v>
       </c>
@@ -2905,13 +2908,13 @@
         <v>45042</v>
       </c>
       <c r="G11" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="I11" s="38" t="s">
         <v>102</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="I11" s="38" t="s">
-        <v>104</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="19" t="s">
@@ -2922,7 +2925,7 @@
       <c r="N11" s="20"/>
       <c r="O11" s="40"/>
     </row>
-    <row r="12" spans="1:15" ht="150.75" thickBot="1">
+    <row r="12" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A12" s="14">
         <v>8</v>
       </c>
@@ -2942,13 +2945,13 @@
         <v>45042</v>
       </c>
       <c r="G12" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" s="18" t="s">
         <v>105</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>107</v>
       </c>
       <c r="J12" s="19"/>
       <c r="K12" s="19" t="s">
@@ -2959,7 +2962,7 @@
       <c r="N12" s="20"/>
       <c r="O12" s="40"/>
     </row>
-    <row r="13" spans="1:15" ht="150.75" thickBot="1">
+    <row r="13" spans="1:15" ht="130.19999999999999" thickBot="1">
       <c r="A13" s="14">
         <v>9</v>
       </c>
@@ -2979,13 +2982,13 @@
         <v>45042</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H13" s="38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I13" s="38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J13" s="19"/>
       <c r="K13" s="19" t="s">
@@ -2996,7 +2999,7 @@
       <c r="N13" s="20"/>
       <c r="O13" s="40"/>
     </row>
-    <row r="14" spans="1:15" ht="120.75" thickBot="1">
+    <row r="14" spans="1:15" ht="202.2" thickBot="1">
       <c r="A14" s="14">
         <v>29</v>
       </c>
@@ -3016,16 +3019,16 @@
         <v>45027</v>
       </c>
       <c r="G14" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="H14" s="38" t="s">
-        <v>97</v>
-      </c>
       <c r="I14" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="K14" s="19" t="s">
         <v>40</v>
@@ -3037,7 +3040,7 @@
       </c>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="1:15" ht="135.75" thickBot="1">
+    <row r="15" spans="1:15" ht="202.2" thickBot="1">
       <c r="A15" s="14">
         <v>37</v>
       </c>
@@ -3057,16 +3060,16 @@
         <v>45027</v>
       </c>
       <c r="G15" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="38" t="s">
-        <v>98</v>
-      </c>
       <c r="I15" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="K15" s="19" t="s">
         <v>40</v>
@@ -3078,7 +3081,7 @@
       </c>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="1:15" ht="90.75" thickBot="1">
+    <row r="16" spans="1:15" ht="202.2" thickBot="1">
       <c r="A16" s="14">
         <v>45</v>
       </c>
@@ -3100,8 +3103,8 @@
       <c r="G16" s="39"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
-      <c r="J16" s="19" t="s">
-        <v>89</v>
+      <c r="J16" s="37" t="s">
+        <v>144</v>
       </c>
       <c r="K16" s="19" t="s">
         <v>40</v>
@@ -3113,7 +3116,7 @@
       </c>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="1:15" ht="120.75" thickBot="1">
+    <row r="17" spans="1:15" ht="331.8" thickBot="1">
       <c r="A17" s="14">
         <v>63</v>
       </c>
@@ -3133,16 +3136,16 @@
         <v>45042</v>
       </c>
       <c r="G17" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="H17" s="38" t="s">
-        <v>111</v>
-      </c>
-      <c r="I17" s="38" t="s">
-        <v>112</v>
-      </c>
       <c r="J17" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>40</v>
@@ -3154,7 +3157,7 @@
       </c>
       <c r="O17" s="40"/>
     </row>
-    <row r="18" spans="1:15" ht="120.75" thickBot="1">
+    <row r="18" spans="1:15" ht="331.8" thickBot="1">
       <c r="A18" s="14">
         <v>64</v>
       </c>
@@ -3174,16 +3177,16 @@
         <v>45042</v>
       </c>
       <c r="G18" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="H18" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="I18" s="38" t="s">
-        <v>115</v>
-      </c>
       <c r="J18" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K18" s="19" t="s">
         <v>40</v>
@@ -3195,7 +3198,7 @@
       </c>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="1:15" ht="120.75" thickBot="1">
+    <row r="19" spans="1:15" ht="331.8" thickBot="1">
       <c r="A19" s="14">
         <v>65</v>
       </c>
@@ -3215,16 +3218,16 @@
         <v>45042</v>
       </c>
       <c r="G19" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="I19" s="38" t="s">
-        <v>118</v>
-      </c>
       <c r="J19" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K19" s="19" t="s">
         <v>40</v>
@@ -3236,7 +3239,7 @@
       </c>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="1:15" ht="120.75" thickBot="1">
+    <row r="20" spans="1:15" ht="331.8" thickBot="1">
       <c r="A20" s="14">
         <v>66</v>
       </c>
@@ -3256,16 +3259,16 @@
         <v>45042</v>
       </c>
       <c r="G20" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="H20" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="I20" s="38" t="s">
-        <v>121</v>
-      </c>
       <c r="J20" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K20" s="37" t="s">
         <v>40</v>
@@ -3277,7 +3280,7 @@
       </c>
       <c r="O20" s="21"/>
     </row>
-    <row r="21" spans="1:15" ht="120.75" thickBot="1">
+    <row r="21" spans="1:15" ht="331.8" thickBot="1">
       <c r="A21" s="14">
         <v>67</v>
       </c>
@@ -3297,16 +3300,16 @@
         <v>45042</v>
       </c>
       <c r="G21" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="H21" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="I21" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="H21" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>124</v>
-      </c>
       <c r="J21" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>40</v>
@@ -3318,7 +3321,7 @@
       </c>
       <c r="O21" s="21"/>
     </row>
-    <row r="22" spans="1:15" ht="120.75" thickBot="1">
+    <row r="22" spans="1:15" ht="331.8" thickBot="1">
       <c r="A22" s="14">
         <v>68</v>
       </c>
@@ -3338,16 +3341,16 @@
         <v>45042</v>
       </c>
       <c r="G22" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="H22" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>127</v>
-      </c>
       <c r="J22" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K22" s="19" t="s">
         <v>40</v>
@@ -3359,7 +3362,7 @@
       </c>
       <c r="O22" s="21"/>
     </row>
-    <row r="23" spans="1:15" ht="120.75" thickBot="1">
+    <row r="23" spans="1:15" ht="331.8" thickBot="1">
       <c r="A23" s="14">
         <v>69</v>
       </c>
@@ -3379,16 +3382,16 @@
         <v>45042</v>
       </c>
       <c r="G23" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="H23" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>130</v>
-      </c>
       <c r="J23" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K23" s="19" t="s">
         <v>40</v>
@@ -3400,7 +3403,7 @@
       </c>
       <c r="O23" s="21"/>
     </row>
-    <row r="24" spans="1:15" ht="120.75" thickBot="1">
+    <row r="24" spans="1:15" ht="331.8" thickBot="1">
       <c r="A24" s="14">
         <v>70</v>
       </c>
@@ -3420,16 +3423,16 @@
         <v>45042</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J24" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K24" s="19" t="s">
         <v>40</v>
@@ -3441,7 +3444,7 @@
       </c>
       <c r="O24" s="21"/>
     </row>
-    <row r="25" spans="1:15" ht="120.75" thickBot="1">
+    <row r="25" spans="1:15" ht="331.8" thickBot="1">
       <c r="A25" s="14">
         <v>71</v>
       </c>
@@ -3461,16 +3464,16 @@
         <v>45042</v>
       </c>
       <c r="G25" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="I25" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="H25" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>135</v>
-      </c>
       <c r="J25" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>40</v>
@@ -3482,7 +3485,7 @@
       </c>
       <c r="O25" s="21"/>
     </row>
-    <row r="26" spans="1:15" ht="120.75" thickBot="1">
+    <row r="26" spans="1:15" ht="331.8" thickBot="1">
       <c r="A26" s="14">
         <v>72</v>
       </c>
@@ -3502,16 +3505,16 @@
         <v>45042</v>
       </c>
       <c r="G26" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="I26" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="H26" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>138</v>
-      </c>
       <c r="J26" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K26" s="19" t="s">
         <v>40</v>
@@ -3523,7 +3526,7 @@
       </c>
       <c r="O26" s="21"/>
     </row>
-    <row r="27" spans="1:15" ht="120.75" thickBot="1">
+    <row r="27" spans="1:15" ht="331.8" thickBot="1">
       <c r="A27" s="14">
         <v>73</v>
       </c>
@@ -3543,16 +3546,16 @@
         <v>45042</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J27" s="37" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
       <c r="K27" s="19" t="s">
         <v>40</v>
@@ -3564,7 +3567,7 @@
       </c>
       <c r="O27" s="21"/>
     </row>
-    <row r="28" spans="1:15" ht="120">
+    <row r="28" spans="1:15" ht="331.2">
       <c r="A28" s="14">
         <v>74</v>
       </c>
@@ -3584,16 +3587,16 @@
         <v>45042</v>
       </c>
       <c r="G28" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I28" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="J28" s="37" t="s">
         <v>142</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="J28" s="37" t="s">
-        <v>91</v>
       </c>
       <c r="K28" s="19" t="s">
         <v>40</v>
@@ -13787,13 +13790,13 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="58.42578125" customWidth="1"/>
-    <col min="5" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="58.44140625" customWidth="1"/>
+    <col min="5" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.25" customHeight="1">
@@ -14897,11 +14900,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>